<commit_message>
AG: grupo y especie
</commit_message>
<xml_diff>
--- a/05_Entregable 3/maate_extra/DdV_19_MAATE_recopilacion_Retenciones.xlsx
+++ b/05_Entregable 3/maate_extra/DdV_19_MAATE_recopilacion_Retenciones.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="10" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="causal_coid_coda_Recopilacion" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,12 @@
     <sheet name="destino_final_Recopilacion" sheetId="11" r:id="rId11"/>
     <sheet name="tipo_proceso_Recopilacion" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="389">
   <si>
     <t>causal_coid_coda</t>
   </si>
@@ -2086,7 +2086,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -2591,16 +2591,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -2608,284 +2610,390 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>385</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>40</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>41</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>42</v>
       </c>
       <c r="B4">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>43</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>44</v>
       </c>
       <c r="B6">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>45</v>
       </c>
       <c r="B7">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>46</v>
       </c>
       <c r="B8">
         <v>177</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>47</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>48</v>
       </c>
       <c r="B10">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>49</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>50</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>51</v>
       </c>
       <c r="B13">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>52</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>53</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>54</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>55</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>56</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>57</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>58</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>59</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>60</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>61</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>62</v>
       </c>
       <c r="B24">
         <v>31</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>63</v>
       </c>
       <c r="B25">
         <v>7</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>64</v>
       </c>
       <c r="B26">
         <v>130</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>65</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>66</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>67</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>68</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>69</v>
       </c>
       <c r="B31">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>70</v>
       </c>
       <c r="B32">
         <v>9</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>71</v>
       </c>
       <c r="B33">
         <v>3</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>72</v>
       </c>
       <c r="B34">
         <v>240</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>73</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>14</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>384</v>
       </c>
     </row>
   </sheetData>
@@ -2898,7 +3006,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C228"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:A15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>